<commit_message>
marine changed to aquatic
</commit_message>
<xml_diff>
--- a/streamlit_wec_full_app_repo/BI_Preliminary_Survey.xlsx
+++ b/streamlit_wec_full_app_repo/BI_Preliminary_Survey.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vishnuvijayasankar/Documents/WEC Convergence Work/streamlit_wec_full_app_repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BEB42C-52F1-CE42-B6C3-CE2C3C8EFB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24A9C8C-3E29-2D49-AC04-01E113B93F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9180" yWindow="4600" windowWidth="27240" windowHeight="16440" xr2:uid="{7FADA319-A0C6-9045-9A61-1F79A7AFF72C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -113,7 +113,7 @@
     <t>Recreational fishing</t>
   </si>
   <si>
-    <t>Marine Space Utilization</t>
+    <t>Aquatic Space Utilization</t>
   </si>
 </sst>
 </file>
@@ -121,7 +121,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -211,29 +211,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -623,7 +623,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>